<commit_message>
added CRUD routes with controllers and models
</commit_message>
<xml_diff>
--- a/capstone_spreadsheet.xlsx
+++ b/capstone_spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>users</t>
   </si>
@@ -51,104 +51,71 @@
     <t xml:space="preserve">color </t>
   </si>
   <si>
-    <t>products</t>
-  </si>
-  <si>
     <t xml:space="preserve">daily_deals </t>
   </si>
   <si>
-    <t>has_many :users</t>
-  </si>
-  <si>
-    <t>coffee_cup</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>12oz</t>
-  </si>
-  <si>
-    <t>shirt</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>short_sleeve</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
-    <t>review</t>
-  </si>
-  <si>
-    <t>great</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>lamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED </t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>bad</t>
-  </si>
-  <si>
     <t>hat</t>
   </si>
   <si>
-    <t>white_sox</t>
-  </si>
-  <si>
-    <t>black</t>
-  </si>
-  <si>
     <t>laptop</t>
   </si>
   <si>
-    <t>macbook_13</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
     <t>shoes</t>
   </si>
   <si>
-    <t>nike_running</t>
-  </si>
-  <si>
-    <t>green/white</t>
-  </si>
-  <si>
     <t xml:space="preserve">has_many :products </t>
   </si>
   <si>
     <t xml:space="preserve">rails g model User          email:string password:string </t>
   </si>
   <si>
-    <t>rails g model DailyDeal user_id:integer name:string description:text price:integer color:string</t>
-  </si>
-  <si>
-    <t>rails g model Product name:string description:text price:integer color:string review:string</t>
-  </si>
-  <si>
     <t>Shopping app that allows a user to find a product with an image and post deals they find</t>
+  </si>
+  <si>
+    <t>white sox baseball logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nike running </t>
+  </si>
+  <si>
+    <t>macbook pro 13in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wish_list </t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>belongs_to :user</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http </t>
+  </si>
+  <si>
+    <t>product_link</t>
+  </si>
+  <si>
+    <t>rails g model Wishlist user_id:integer product_link:string</t>
+  </si>
+  <si>
+    <t>rails g model DailyDeal user_id:integer name:string description:text price:integer color:string product_link:string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,6 +148,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -210,10 +183,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -547,31 +522,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -582,203 +559,169 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
+      <c r="E16">
+        <v>1000</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1">
+      <c r="A22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="1" customFormat="1">
-      <c r="A24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25">
-        <v>31</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26">
-        <v>32</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26">
-        <v>1000</v>
-      </c>
-      <c r="F26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27">
-        <v>33</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27">
-        <v>60</v>
-      </c>
-      <c r="F27" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>